<commit_message>
6th Commit #Loginbanner Configuration
6th Commit #Loginbanner Configuration
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -5,20 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.6.206\Users\yadhukrishnan.p\Documents\GitHub\BeaconFCM_SJ\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megha.zarkar\Documents\GitHub\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D61D751-C645-4FBF-A4C3-6BB0101AF39E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CDE48C-DC22-440D-AF1F-518FA1D33DDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="1" activeTab="3" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16050" windowHeight="3780" tabRatio="597" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Disposition_master" sheetId="3" r:id="rId1"/>
-    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId2"/>
-    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId3"/>
-    <sheet name="CoreUserManagement" sheetId="6" r:id="rId4"/>
+    <sheet name="Login_banner_confi" sheetId="8" r:id="rId1"/>
+    <sheet name="Disposition_master" sheetId="3" r:id="rId2"/>
+    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId3"/>
+    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId4"/>
+    <sheet name="CoreUserManagement" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="128">
   <si>
     <t>Run</t>
   </si>
@@ -247,15 +249,6 @@
     <t>NumberEightDigits</t>
   </si>
   <si>
-    <t>AlphabeticInputName</t>
-  </si>
-  <si>
-    <t>NumericInputName</t>
-  </si>
-  <si>
-    <t>AlphaNumericInputName</t>
-  </si>
-  <si>
     <t>ZoneCo</t>
   </si>
   <si>
@@ -338,6 +331,102 @@
   </si>
   <si>
     <t>test@123</t>
+  </si>
+  <si>
+    <t>AlphaNumericInput</t>
+  </si>
+  <si>
+    <t>Login_banner_confi</t>
+  </si>
+  <si>
+    <t>NumtName</t>
+  </si>
+  <si>
+    <t>nputName</t>
+  </si>
+  <si>
+    <t>TestAutomation1001</t>
+  </si>
+  <si>
+    <t>HeadingField</t>
+  </si>
+  <si>
+    <t>DetailField</t>
+  </si>
+  <si>
+    <t>Detailfield1link</t>
+  </si>
+  <si>
+    <t>Headerfield1link</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/</t>
+  </si>
+  <si>
+    <t>Link_1</t>
+  </si>
+  <si>
+    <t>Modifiedlink1</t>
+  </si>
+  <si>
+    <t>https://www.grammarly.com/</t>
+  </si>
+  <si>
+    <t>Header10</t>
+  </si>
+  <si>
+    <t>Detail10</t>
+  </si>
+  <si>
+    <t>CallCenterHeadingtext</t>
+  </si>
+  <si>
+    <t>CallCenterDetailtext</t>
+  </si>
+  <si>
+    <t>CallCenterDetailLink1</t>
+  </si>
+  <si>
+    <t>https://www.zoho.com/calendar/personal-calendar.html</t>
+  </si>
+  <si>
+    <t>CallCenterHeaderLink1</t>
+  </si>
+  <si>
+    <t>CallCentre01</t>
+  </si>
+  <si>
+    <t>CallCenterModifiedHeader</t>
+  </si>
+  <si>
+    <t>CallCenterModifiedDetail</t>
+  </si>
+  <si>
+    <t>CallCentre</t>
+  </si>
+  <si>
+    <t>https://chatgpt.com/</t>
+  </si>
+  <si>
+    <t>AgencyUserHeader1</t>
+  </si>
+  <si>
+    <t>AgencyUserDetail1</t>
+  </si>
+  <si>
+    <t>AgencyHeader1</t>
+  </si>
+  <si>
+    <t>AgencyDetails1</t>
+  </si>
+  <si>
+    <t>AgencyUpdatedHeader1</t>
+  </si>
+  <si>
+    <t>AgencyUpdatedDetail1</t>
+  </si>
+  <si>
+    <t>Agency header_1</t>
   </si>
 </sst>
 </file>
@@ -452,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -515,6 +604,24 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -830,38 +937,190 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B96A424-403E-4AFF-A0B1-66754F421E3B}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" customWidth="1"/>
+    <col min="15" max="15" width="7" customWidth="1"/>
+    <col min="16" max="16" width="3.42578125" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" customWidth="1"/>
+    <col min="18" max="18" width="26.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="29" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="O2" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q2" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="R2" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{D27CA4DC-DA2A-4D0C-B827-EC20B413DB73}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{D963CC3E-5A70-4A75-BE61-2F2D816054E7}"/>
+    <hyperlink ref="N2" r:id="rId3" xr:uid="{3AAEDCFB-544C-440B-95FB-43316F12D8E0}"/>
+    <hyperlink ref="R2" r:id="rId4" xr:uid="{8CB32D9B-99C5-4E49-A190-E25427AF09F8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067DCD9D-336F-4B7B-9363-04AE9D95019D}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="45.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="40.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -923,7 +1182,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -990,28 +1249,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F19261-6837-44AB-8CDF-ACF0A2220A25}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1046,7 +1305,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1087,7 +1346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCC895A-2382-45F5-A8F1-2814E48093FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1095,15 +1354,15 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.54296875" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1120,7 +1379,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1142,41 +1401,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD0DAF-92F9-4A53-BD4C-11CDE669575B}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1223,117 +1484,117 @@
         <v>67</v>
       </c>
       <c r="P1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="S1" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="T1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="U1" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="V1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="T1" s="18" t="s">
+      <c r="W1" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="X1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="V1" s="18" t="s">
+      <c r="Y1" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="Z1" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="X1" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y1" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z1" s="18" t="s">
-        <v>78</v>
-      </c>
     </row>
-    <row r="2" spans="1:26" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E2" s="19">
         <v>8089889900</v>
       </c>
       <c r="F2" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="L2" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="M2" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="19" t="s">
+      <c r="N2" s="19" t="s">
         <v>85</v>
-      </c>
-      <c r="L2" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="M2" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="N2" s="19" t="s">
-        <v>88</v>
       </c>
       <c r="O2" s="19">
         <v>90089257</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="Q2" s="19">
         <v>12345</v>
       </c>
       <c r="R2" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="S2" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="T2" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="U2" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="S2" s="19" t="s">
+      <c r="V2" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="T2" s="19" t="s">
+      <c r="W2" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="U2" s="19" t="s">
+      <c r="X2" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="V2" s="19" t="s">
+      <c r="Y2" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="W2" s="19" t="s">
+      <c r="Z2" s="26" t="s">
         <v>95</v>
-      </c>
-      <c r="X2" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y2" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z2" s="26" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1344,4 +1605,16 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5BD2CE4-FC5B-4B49-8E15-DE33886DCDDC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
7th Commit #Login Banner Configuration
7th Commit #Login Banner Configuration
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megha.zarkar\Documents\GitHub\BeaconFCM_SJ\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CDE48C-DC22-440D-AF1F-518FA1D33DDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8C9156C9-B44D-4941-A0DD-54D07F9C0E04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16050" windowHeight="3780" tabRatio="597" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12450" windowHeight="3720" tabRatio="597" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_banner_confi" sheetId="8" r:id="rId1"/>
@@ -21,6 +16,7 @@
     <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -360,9 +356,6 @@
     <t>Headerfield1link</t>
   </si>
   <si>
-    <t>https://www.w3schools.com/</t>
-  </si>
-  <si>
     <t>Link_1</t>
   </si>
   <si>
@@ -427,6 +420,9 @@
   </si>
   <si>
     <t>Agency header_1</t>
+  </si>
+  <si>
+    <t>https://www.google.com/</t>
   </si>
 </sst>
 </file>
@@ -614,14 +610,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -940,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B96A424-403E-4AFF-A0B1-66754F421E3B}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,11 +946,11 @@
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="4" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" customWidth="1"/>
     <col min="11" max="11" width="7.85546875" customWidth="1"/>
     <col min="12" max="12" width="13.7109375" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" customWidth="1"/>
@@ -988,37 +984,37 @@
         <v>103</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I1" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="K1" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>113</v>
-      </c>
       <c r="M1" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="N1" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="N1" s="21" t="s">
-        <v>118</v>
-      </c>
       <c r="O1" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="P1" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="P1" s="21" t="s">
-        <v>122</v>
-      </c>
       <c r="Q1" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="R1" s="21" t="s">
         <v>125</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="29" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -1029,52 +1025,52 @@
         <v>2</v>
       </c>
       <c r="C2" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>109</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>110</v>
       </c>
       <c r="E2" s="27" t="s">
         <v>100</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="31" t="s">
-        <v>108</v>
+      <c r="G2" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>107</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J2" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>114</v>
+        <v>105</v>
+      </c>
+      <c r="L2" s="31" t="s">
+        <v>113</v>
       </c>
       <c r="M2" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="N2" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="N2" s="32" t="s">
-        <v>120</v>
-      </c>
       <c r="O2" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="P2" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="P2" s="27" t="s">
-        <v>124</v>
-      </c>
       <c r="Q2" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="R2" s="31" t="s">
-        <v>108</v>
+        <v>126</v>
+      </c>
+      <c r="R2" s="30" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1083,6 +1079,7 @@
     <hyperlink ref="L2" r:id="rId2" xr:uid="{D963CC3E-5A70-4A75-BE61-2F2D816054E7}"/>
     <hyperlink ref="N2" r:id="rId3" xr:uid="{3AAEDCFB-544C-440B-95FB-43316F12D8E0}"/>
     <hyperlink ref="R2" r:id="rId4" xr:uid="{8CB32D9B-99C5-4E49-A190-E25427AF09F8}"/>
+    <hyperlink ref="G2" r:id="rId5" xr:uid="{7B3B365C-A6FD-475D-BA81-BBA727EA0EB0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
12th commit - Changes in collection agency add new agent and agent list tc
12th commit - Changes in collection agency add new agent and agent list tc
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.6.206\Users\yadhukrishnan.p\Documents\GitHub\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA05E5B-7AE5-4087-B12B-3E73BD609970}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3289D280-07D1-47BF-80DB-D7921E7AC7D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="2" activeTab="4" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13100" windowHeight="3770" firstSheet="3" activeTab="5" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Disposition_master" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId3"/>
     <sheet name="CoreUserManagement" sheetId="6" r:id="rId4"/>
     <sheet name="CoreHOUserCreation" sheetId="7" r:id="rId5"/>
+    <sheet name="CA-AddNewAgent" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="103">
   <si>
     <t>Run</t>
   </si>
@@ -345,6 +346,12 @@
   </si>
   <si>
     <t>docstra@gmail.com</t>
+  </si>
+  <si>
+    <t>Collection Agency Agent management Add new agent and agent list</t>
+  </si>
+  <si>
+    <t>muthoot4</t>
   </si>
 </sst>
 </file>
@@ -1371,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1090DB4-E483-4C4D-8367-1410BDACF1EB}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1438,4 +1445,52 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB84F0AE-8762-4FD5-92CA-A4BB37675E67}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.08984375" customWidth="1"/>
+    <col min="4" max="4" width="17.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
13th commit - Core regularization summary TC by pinku
13th commit - Core regularization summary TC by pinku
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.6.206\Users\yadhukrishnan.p\Documents\GitHub\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3289D280-07D1-47BF-80DB-D7921E7AC7D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D06BBB0-280B-4F99-951F-F4F7D85B6694}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13100" windowHeight="3770" firstSheet="3" activeTab="5" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13100" windowHeight="3770" firstSheet="4" activeTab="6" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Disposition_master" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="CoreUserManagement" sheetId="6" r:id="rId4"/>
     <sheet name="CoreHOUserCreation" sheetId="7" r:id="rId5"/>
     <sheet name="CA-AddNewAgent" sheetId="8" r:id="rId6"/>
+    <sheet name="Core_Regularization_Summary" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="111">
   <si>
     <t>Run</t>
   </si>
@@ -352,6 +353,30 @@
   </si>
   <si>
     <t>muthoot4</t>
+  </si>
+  <si>
+    <t>OutstandingBalanceOperator</t>
+  </si>
+  <si>
+    <t>OutstandingBalance</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>AllocateTo</t>
+  </si>
+  <si>
+    <t>SelectCallCentre</t>
+  </si>
+  <si>
+    <t>Core_Regularization_Summary</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>CallCentre 1</t>
   </si>
 </sst>
 </file>
@@ -466,7 +491,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -541,6 +566,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1451,7 +1488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB84F0AE-8762-4FD5-92CA-A4BB37675E67}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1493,4 +1530,74 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89943E99-F0EA-477A-BC49-972CD3C95FD8}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27" style="28" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="28"/>
+    <col min="3" max="3" width="25.7265625" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.81640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="33">
+        <v>25000</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2nd commit #Agency Account Allocation
2nd commit #Agency Account Allocation
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,20 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8C9156C9-B44D-4941-A0DD-54D07F9C0E04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megha.zarkar\Documents\GitHub\BeaconFCM_SJ\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29B220B-004F-4CEB-9091-A4AD7C6E66F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12450" windowHeight="3720" tabRatio="597" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15930" windowHeight="2805" tabRatio="597" activeTab="2" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_banner_confi" sheetId="8" r:id="rId1"/>
     <sheet name="Disposition_master" sheetId="3" r:id="rId2"/>
-    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId3"/>
-    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId4"/>
-    <sheet name="CoreUserManagement" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
+    <sheet name="Agency_Account_Allocation" sheetId="10" r:id="rId3"/>
+    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId4"/>
+    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId5"/>
+    <sheet name="CoreUserManagement" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="130">
   <si>
     <t>Run</t>
   </si>
@@ -423,6 +428,12 @@
   </si>
   <si>
     <t>https://www.google.com/</t>
+  </si>
+  <si>
+    <t>DPD</t>
+  </si>
+  <si>
+    <t>Agency_Account_Allocation</t>
   </si>
 </sst>
 </file>
@@ -936,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B96A424-403E-4AFF-A0B1-66754F421E3B}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,7 +1028,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="29" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="29" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>97</v>
       </c>
@@ -1089,7 +1100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067DCD9D-336F-4B7B-9363-04AE9D95019D}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
@@ -1247,11 +1258,53 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52ABB169-42AE-4B07-BC37-495C3DAF74AB}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29">
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F19261-6837-44AB-8CDF-ACF0A2220A25}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,7 +1396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCC895A-2382-45F5-A8F1-2814E48093FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1398,7 +1451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD0DAF-92F9-4A53-BD4C-11CDE669575B}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
@@ -1604,7 +1657,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5BD2CE4-FC5B-4B49-8E15-DE33886DCDDC}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
22nd commit - Call centre role management by neha
22nd commit - Call centre role management by neha
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.6.206\Users\yadhukrishnan.p\Documents\GitHub\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CF14A9-A914-4ED6-A308-BB1854791BC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D8F08E-5A7A-43FB-A829-8C4FFB43C3B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="7" activeTab="9" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Disposition_master" sheetId="3" r:id="rId1"/>
-    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId2"/>
-    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId3"/>
-    <sheet name="CoreUserManagement" sheetId="6" r:id="rId4"/>
-    <sheet name="CoreHOUserCreation" sheetId="7" r:id="rId5"/>
-    <sheet name="CA-AddNewAgent" sheetId="8" r:id="rId6"/>
-    <sheet name="Core_Regularization_Summary" sheetId="9" r:id="rId7"/>
-    <sheet name="CollectionAgencyDisposition" sheetId="10" r:id="rId8"/>
-    <sheet name="CA-AgentAccountAllocation" sheetId="11" r:id="rId9"/>
-    <sheet name="Core_LoginBannerConfig" sheetId="12" r:id="rId10"/>
+    <sheet name="CallCentreRoleManagement" sheetId="13" r:id="rId2"/>
+    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId3"/>
+    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId4"/>
+    <sheet name="CoreUserManagement" sheetId="6" r:id="rId5"/>
+    <sheet name="CoreHOUserCreation" sheetId="7" r:id="rId6"/>
+    <sheet name="CA-AddNewAgent" sheetId="8" r:id="rId7"/>
+    <sheet name="Core_Regularization_Summary" sheetId="9" r:id="rId8"/>
+    <sheet name="CollectionAgencyDisposition" sheetId="10" r:id="rId9"/>
+    <sheet name="CA-AgentAccountAllocation" sheetId="11" r:id="rId10"/>
+    <sheet name="Core_LoginBannerConfig" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="164">
   <si>
     <t>Run</t>
   </si>
@@ -533,6 +534,12 @@
   </si>
   <si>
     <t>Agency header_1</t>
+  </si>
+  <si>
+    <t>CallCenter</t>
+  </si>
+  <si>
+    <t>yuki4</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1108,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1258,10 +1265,99 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502A90A9-AB89-4C76-BF21-0726E83DFEAA}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.90625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="J1" s="45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="44">
+        <v>10</v>
+      </c>
+      <c r="J2" s="47">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319A2FA0-C188-4BFC-B422-FA837B3784A7}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -1412,6 +1508,49 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63FFAB67-A0F2-4F57-B685-B5FFC2EC3004}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F19261-6837-44AB-8CDF-ACF0A2220A25}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1508,7 +1647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCC895A-2382-45F5-A8F1-2814E48093FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1563,7 +1702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD0DAF-92F9-4A53-BD4C-11CDE669575B}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
@@ -1769,7 +1908,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1090DB4-E483-4C4D-8367-1410BDACF1EB}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1842,7 +1981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB84F0AE-8762-4FD5-92CA-A4BB37675E67}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1890,7 +2029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89943E99-F0EA-477A-BC49-972CD3C95FD8}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1960,7 +2099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE214A7F-1CCD-473B-9D90-2C8A2FFCDD67}">
   <dimension ref="A1:S2"/>
   <sheetViews>
@@ -2100,93 +2239,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502A90A9-AB89-4C76-BF21-0726E83DFEAA}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="33.90625" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="G1" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="I1" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="J1" s="45" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="D2" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="F2" s="46" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="I2" s="44">
-        <v>10</v>
-      </c>
-      <c r="J2" s="47">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
25th commit - Core alerts mask account and mask authorization, New listener
25th commit - Core alerts mask account and mask authorization, New listener
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.6.206\Users\yadhukrishnan.p\Documents\GitHub\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31094F2-7271-4E83-889D-714B45E119EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B881E1A-AB50-436D-A423-31BD014A96C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="3" activeTab="4" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="4" activeTab="5" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Disposition_master" sheetId="3" r:id="rId1"/>
@@ -18,15 +18,16 @@
     <sheet name="CoreAlertsPlaceholderManagement" sheetId="14" r:id="rId3"/>
     <sheet name="AlertsTemplateManagement" sheetId="15" r:id="rId4"/>
     <sheet name="AlertsNotificationManagement" sheetId="16" r:id="rId5"/>
-    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId6"/>
-    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId7"/>
-    <sheet name="CoreUserManagement" sheetId="6" r:id="rId8"/>
-    <sheet name="CoreHOUserCreation" sheetId="7" r:id="rId9"/>
-    <sheet name="CA-AddNewAgent" sheetId="8" r:id="rId10"/>
-    <sheet name="Core_Regularization_Summary" sheetId="9" r:id="rId11"/>
-    <sheet name="CollectionAgencyDisposition" sheetId="10" r:id="rId12"/>
-    <sheet name="CA-AgentAccountAllocation" sheetId="11" r:id="rId13"/>
-    <sheet name="Core_LoginBannerConfig" sheetId="12" r:id="rId14"/>
+    <sheet name="CoreAlertsMaskAcAndMaskingAutho" sheetId="17" r:id="rId6"/>
+    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId7"/>
+    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId8"/>
+    <sheet name="CoreUserManagement" sheetId="6" r:id="rId9"/>
+    <sheet name="CoreHOUserCreation" sheetId="7" r:id="rId10"/>
+    <sheet name="CA-AddNewAgent" sheetId="8" r:id="rId11"/>
+    <sheet name="Core_Regularization_Summary" sheetId="9" r:id="rId12"/>
+    <sheet name="CollectionAgencyDisposition" sheetId="10" r:id="rId13"/>
+    <sheet name="CA-AgentAccountAllocation" sheetId="11" r:id="rId14"/>
+    <sheet name="Core_LoginBannerConfig" sheetId="12" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="195">
   <si>
     <t>Run</t>
   </si>
@@ -612,6 +613,30 @@
   </si>
   <si>
     <t>One Time</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>Status2</t>
+  </si>
+  <si>
+    <t>CoreAlertsMaskAcAndMaskingAutho</t>
+  </si>
+  <si>
+    <t>Mask</t>
+  </si>
+  <si>
+    <t>Email 2</t>
+  </si>
+  <si>
+    <t>Unmask</t>
   </si>
 </sst>
 </file>
@@ -1360,6 +1385,79 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1090DB4-E483-4C4D-8367-1410BDACF1EB}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="20">
+        <v>8089889900</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{C19478ED-D9C8-4F47-8F0B-F1D58C09B34B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB84F0AE-8762-4FD5-92CA-A4BB37675E67}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1407,7 +1505,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89943E99-F0EA-477A-BC49-972CD3C95FD8}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1477,7 +1575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE214A7F-1CCD-473B-9D90-2C8A2FFCDD67}">
   <dimension ref="A1:S2"/>
   <sheetViews>
@@ -1619,7 +1717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502A90A9-AB89-4C76-BF21-0726E83DFEAA}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -1708,7 +1806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319A2FA0-C188-4BFC-B422-FA837B3784A7}">
   <dimension ref="A1:R2"/>
   <sheetViews>
@@ -2038,8 +2136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60AF55B7-F436-43C5-9963-D938C7EFC65D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2076,6 +2174,76 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08976CF2-4030-41C6-895D-319E753EDB55}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="36.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>190</v>
+      </c>
+      <c r="H1" s="57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" s="56" t="s">
+        <v>193</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>194</v>
+      </c>
+      <c r="H2" s="56">
+        <v>1234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F19261-6837-44AB-8CDF-ACF0A2220A25}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -2172,7 +2340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCC895A-2382-45F5-A8F1-2814E48093FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2227,7 +2395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD0DAF-92F9-4A53-BD4C-11CDE669575B}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
@@ -2431,77 +2599,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1090DB4-E483-4C4D-8367-1410BDACF1EB}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.90625" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="20">
-        <v>8089889900</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{C19478ED-D9C8-4F47-8F0B-F1D58C09B34B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
1st Commit #View Template List
1st Commit #View Template List
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megha.zarkar\Documents\GitHub\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29B220B-004F-4CEB-9091-A4AD7C6E66F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5438D6-52F7-4C91-974F-82DB4982F06F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15930" windowHeight="2805" tabRatio="597" activeTab="2" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15930" windowHeight="2805" tabRatio="597" activeTab="3" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_banner_confi" sheetId="8" r:id="rId1"/>
     <sheet name="Disposition_master" sheetId="3" r:id="rId2"/>
     <sheet name="Agency_Account_Allocation" sheetId="10" r:id="rId3"/>
-    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId4"/>
-    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId5"/>
-    <sheet name="CoreUserManagement" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
+    <sheet name="ViewTemplateList" sheetId="11" r:id="rId4"/>
+    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId5"/>
+    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId6"/>
+    <sheet name="CoreUserManagement" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="135">
   <si>
     <t>Run</t>
   </si>
@@ -434,6 +435,21 @@
   </si>
   <si>
     <t>Agency_Account_Allocation</t>
+  </si>
+  <si>
+    <t>View_Template_List</t>
+  </si>
+  <si>
+    <t>Template Name</t>
+  </si>
+  <si>
+    <t>Sample Template</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Q1</t>
   </si>
 </sst>
 </file>
@@ -1261,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52ABB169-42AE-4B07-BC37-495C3DAF74AB}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,6 +1316,54 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280FE8FD-D2BB-4A01-A509-A942B9BAD8DD}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F19261-6837-44AB-8CDF-ACF0A2220A25}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1396,7 +1460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCC895A-2382-45F5-A8F1-2814E48093FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1451,7 +1515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD0DAF-92F9-4A53-BD4C-11CDE669575B}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
@@ -1657,7 +1721,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5BD2CE4-FC5B-4B49-8E15-DE33886DCDDC}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
26th commit - Core bank allocation summary and Core agent account allocation
26th commit - Core bank allocation summary and Core agent account allocation
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.6.206\Users\yadhukrishnan.p\Documents\GitHub\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B881E1A-AB50-436D-A423-31BD014A96C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04CF3EC-8F86-4D43-8FE5-9CC5ED917663}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="4" activeTab="5" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="6" activeTab="7" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Disposition_master" sheetId="3" r:id="rId1"/>
@@ -19,15 +19,17 @@
     <sheet name="AlertsTemplateManagement" sheetId="15" r:id="rId4"/>
     <sheet name="AlertsNotificationManagement" sheetId="16" r:id="rId5"/>
     <sheet name="CoreAlertsMaskAcAndMaskingAutho" sheetId="17" r:id="rId6"/>
-    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId7"/>
-    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId8"/>
-    <sheet name="CoreUserManagement" sheetId="6" r:id="rId9"/>
-    <sheet name="CoreHOUserCreation" sheetId="7" r:id="rId10"/>
-    <sheet name="CA-AddNewAgent" sheetId="8" r:id="rId11"/>
-    <sheet name="Core_Regularization_Summary" sheetId="9" r:id="rId12"/>
-    <sheet name="CollectionAgencyDisposition" sheetId="10" r:id="rId13"/>
-    <sheet name="CA-AgentAccountAllocation" sheetId="11" r:id="rId14"/>
-    <sheet name="Core_LoginBannerConfig" sheetId="12" r:id="rId15"/>
+    <sheet name="AgentAccountAllocation" sheetId="18" r:id="rId7"/>
+    <sheet name="CoreBankAllocationSummary" sheetId="19" r:id="rId8"/>
+    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId9"/>
+    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId10"/>
+    <sheet name="CoreUserManagement" sheetId="6" r:id="rId11"/>
+    <sheet name="CoreHOUserCreation" sheetId="7" r:id="rId12"/>
+    <sheet name="CA-AddNewAgent" sheetId="8" r:id="rId13"/>
+    <sheet name="Core_Regularization_Summary" sheetId="9" r:id="rId14"/>
+    <sheet name="CollectionAgencyDisposition" sheetId="10" r:id="rId15"/>
+    <sheet name="CA-AgentAccountAllocation" sheetId="11" r:id="rId16"/>
+    <sheet name="Core_LoginBannerConfig" sheetId="12" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="202">
   <si>
     <t>Run</t>
   </si>
@@ -637,6 +639,27 @@
   </si>
   <si>
     <t>Unmask</t>
+  </si>
+  <si>
+    <t>DPD</t>
+  </si>
+  <si>
+    <t>Agency_Account_Allocation</t>
+  </si>
+  <si>
+    <t>OsBalanceOperator</t>
+  </si>
+  <si>
+    <t>OsBalanceAmount</t>
+  </si>
+  <si>
+    <t>CoreBankAllocationSummary</t>
+  </si>
+  <si>
+    <t>Amaravati</t>
+  </si>
+  <si>
+    <t>&lt;</t>
   </si>
 </sst>
 </file>
@@ -757,7 +780,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -909,6 +932,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1385,962 +1411,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1090DB4-E483-4C4D-8367-1410BDACF1EB}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.90625" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="20">
-        <v>8089889900</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{C19478ED-D9C8-4F47-8F0B-F1D58C09B34B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB84F0AE-8762-4FD5-92CA-A4BB37675E67}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.08984375" customWidth="1"/>
-    <col min="4" max="4" width="17.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89943E99-F0EA-477A-BC49-972CD3C95FD8}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="27" style="28" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="28"/>
-    <col min="3" max="3" width="25.7265625" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.81640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" style="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="28"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="33">
-        <v>25000</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>110</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE214A7F-1CCD-473B-9D90-2C8A2FFCDD67}">
-  <dimension ref="A1:S2"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="21" style="37" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="37"/>
-    <col min="3" max="3" width="14" style="37" customWidth="1"/>
-    <col min="4" max="4" width="13.90625" style="37" customWidth="1"/>
-    <col min="5" max="18" width="8.7265625" style="37"/>
-    <col min="19" max="19" width="18.7265625" style="37" customWidth="1"/>
-    <col min="20" max="16384" width="8.7265625" style="37"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="J1" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="M1" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="N1" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="O1" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="P1" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q1" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="R1" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" s="36" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="38">
-        <v>25000</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="H2" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="I2" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="J2" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="K2" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="L2" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="M2" s="38">
-        <v>10</v>
-      </c>
-      <c r="N2" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="O2" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="P2" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q2" s="40">
-        <v>18</v>
-      </c>
-      <c r="R2" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" s="38">
-        <v>1000000000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502A90A9-AB89-4C76-BF21-0726E83DFEAA}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="33.90625" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="G1" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="I1" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="J1" s="45" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="D2" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="F2" s="46" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="I2" s="44">
-        <v>10</v>
-      </c>
-      <c r="J2" s="47">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319A2FA0-C188-4BFC-B422-FA837B3784A7}">
-  <dimension ref="A1:R2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="F1" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="G1" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="H1" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="I1" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="J1" s="42" t="s">
-        <v>139</v>
-      </c>
-      <c r="K1" s="42" t="s">
-        <v>140</v>
-      </c>
-      <c r="L1" s="42" t="s">
-        <v>141</v>
-      </c>
-      <c r="M1" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="N1" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="O1" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="P1" s="42" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q1" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="R1" s="42" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="E2" s="48" t="s">
-        <v>151</v>
-      </c>
-      <c r="F2" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="G2" s="50" t="s">
-        <v>153</v>
-      </c>
-      <c r="H2" s="51" t="s">
-        <v>154</v>
-      </c>
-      <c r="I2" s="49" t="s">
-        <v>155</v>
-      </c>
-      <c r="J2" s="48" t="s">
-        <v>155</v>
-      </c>
-      <c r="K2" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="L2" s="52" t="s">
-        <v>156</v>
-      </c>
-      <c r="M2" s="48" t="s">
-        <v>157</v>
-      </c>
-      <c r="N2" s="52" t="s">
-        <v>158</v>
-      </c>
-      <c r="O2" s="48" t="s">
-        <v>159</v>
-      </c>
-      <c r="P2" s="48" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q2" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="R2" s="51" t="s">
-        <v>154</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{8328FD81-C02A-4C0F-950B-6B9A8614EF57}"/>
-    <hyperlink ref="L2" r:id="rId2" xr:uid="{286913B0-9B53-4832-AC16-513CA5856665}"/>
-    <hyperlink ref="N2" r:id="rId3" xr:uid="{1F70C33F-508E-437B-84BC-4B0B4B5ED4E3}"/>
-    <hyperlink ref="R2" r:id="rId4" xr:uid="{34D533E6-04E8-488B-BF9A-CA683DEE4EB3}"/>
-    <hyperlink ref="G2" r:id="rId5" xr:uid="{E9AEAAD2-9D32-47F8-BBE3-33FF8277F014}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63FFAB67-A0F2-4F57-B685-B5FFC2EC3004}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B87CED1-ADCF-4939-B0CC-BC7CD7B25447}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="42.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="54" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
-        <v>164</v>
-      </c>
-      <c r="B2" s="55" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96D56B6-4C74-412E-B95B-21C862046E92}">
-  <dimension ref="A1:L2"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="24.6328125" customWidth="1"/>
-    <col min="10" max="10" width="65.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="57" t="s">
-        <v>165</v>
-      </c>
-      <c r="D1" s="57" t="s">
-        <v>166</v>
-      </c>
-      <c r="E1" s="57" t="s">
-        <v>167</v>
-      </c>
-      <c r="F1" s="57" t="s">
-        <v>168</v>
-      </c>
-      <c r="G1" s="57" t="s">
-        <v>169</v>
-      </c>
-      <c r="H1" s="57" t="s">
-        <v>170</v>
-      </c>
-      <c r="I1" s="57" t="s">
-        <v>171</v>
-      </c>
-      <c r="J1" s="57" t="s">
-        <v>172</v>
-      </c>
-      <c r="K1" s="57" t="s">
-        <v>173</v>
-      </c>
-      <c r="L1" s="57" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="B2" s="55" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>177</v>
-      </c>
-      <c r="E2" s="56" t="s">
-        <v>178</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>179</v>
-      </c>
-      <c r="G2" s="56" t="s">
-        <v>177</v>
-      </c>
-      <c r="H2" s="56" t="s">
-        <v>180</v>
-      </c>
-      <c r="I2" s="56" t="s">
-        <v>181</v>
-      </c>
-      <c r="J2" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="K2" s="56" t="s">
-        <v>183</v>
-      </c>
-      <c r="L2" s="56" t="s">
-        <v>181</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60AF55B7-F436-43C5-9963-D938C7EFC65D}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="57" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
-        <v>185</v>
-      </c>
-      <c r="B2" s="55" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>186</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08976CF2-4030-41C6-895D-319E753EDB55}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="36.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="57" t="s">
-        <v>187</v>
-      </c>
-      <c r="D1" s="57" t="s">
-        <v>188</v>
-      </c>
-      <c r="E1" s="57" t="s">
-        <v>165</v>
-      </c>
-      <c r="F1" s="57" t="s">
-        <v>189</v>
-      </c>
-      <c r="G1" s="57" t="s">
-        <v>190</v>
-      </c>
-      <c r="H1" s="57" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" s="55" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="D2" s="56" t="s">
-        <v>181</v>
-      </c>
-      <c r="E2" s="56" t="s">
-        <v>179</v>
-      </c>
-      <c r="F2" s="56" t="s">
-        <v>193</v>
-      </c>
-      <c r="G2" s="56" t="s">
-        <v>194</v>
-      </c>
-      <c r="H2" s="56">
-        <v>1234</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F19261-6837-44AB-8CDF-ACF0A2220A25}">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="13">
-        <v>1.23456789012345E+28</v>
-      </c>
-      <c r="E2" s="15">
-        <v>1.23123212312321E+24</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="12">
-        <v>18</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" s="17">
-        <v>45644</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCC895A-2382-45F5-A8F1-2814E48093FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2395,7 +1465,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD0DAF-92F9-4A53-BD4C-11CDE669575B}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
@@ -2599,4 +1669,1083 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1090DB4-E483-4C4D-8367-1410BDACF1EB}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="20">
+        <v>8089889900</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{C19478ED-D9C8-4F47-8F0B-F1D58C09B34B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB84F0AE-8762-4FD5-92CA-A4BB37675E67}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.08984375" customWidth="1"/>
+    <col min="4" max="4" width="17.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89943E99-F0EA-477A-BC49-972CD3C95FD8}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27" style="28" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="28"/>
+    <col min="3" max="3" width="25.7265625" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.81640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="33">
+        <v>25000</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE214A7F-1CCD-473B-9D90-2C8A2FFCDD67}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21" style="37" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="37"/>
+    <col min="3" max="3" width="14" style="37" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" style="37" customWidth="1"/>
+    <col min="5" max="18" width="8.7265625" style="37"/>
+    <col min="19" max="19" width="18.7265625" style="37" customWidth="1"/>
+    <col min="20" max="16384" width="8.7265625" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q1" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="R1" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" s="36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="38">
+        <v>25000</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="L2" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" s="38">
+        <v>10</v>
+      </c>
+      <c r="N2" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="O2" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="P2" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q2" s="40">
+        <v>18</v>
+      </c>
+      <c r="R2" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="38">
+        <v>1000000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502A90A9-AB89-4C76-BF21-0726E83DFEAA}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.90625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="J1" s="45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="44">
+        <v>10</v>
+      </c>
+      <c r="J2" s="47">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319A2FA0-C188-4BFC-B422-FA837B3784A7}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="L1" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="M1" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="N1" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="O1" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="P1" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q1" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="R1" s="42" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" s="50" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="51" t="s">
+        <v>154</v>
+      </c>
+      <c r="I2" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="J2" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="L2" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="M2" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="N2" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="O2" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="P2" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q2" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="R2" s="51" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{8328FD81-C02A-4C0F-950B-6B9A8614EF57}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{286913B0-9B53-4832-AC16-513CA5856665}"/>
+    <hyperlink ref="N2" r:id="rId3" xr:uid="{1F70C33F-508E-437B-84BC-4B0B4B5ED4E3}"/>
+    <hyperlink ref="R2" r:id="rId4" xr:uid="{34D533E6-04E8-488B-BF9A-CA683DEE4EB3}"/>
+    <hyperlink ref="G2" r:id="rId5" xr:uid="{E9AEAAD2-9D32-47F8-BBE3-33FF8277F014}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63FFAB67-A0F2-4F57-B685-B5FFC2EC3004}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B87CED1-ADCF-4939-B0CC-BC7CD7B25447}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="42.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="53" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96D56B6-4C74-412E-B95B-21C862046E92}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.6328125" customWidth="1"/>
+    <col min="10" max="10" width="65.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" s="57" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1" s="57" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" s="57" t="s">
+        <v>173</v>
+      </c>
+      <c r="L1" s="57" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="53" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="H2" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="I2" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="J2" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="K2" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="L2" s="56" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60AF55B7-F436-43C5-9963-D938C7EFC65D}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08976CF2-4030-41C6-895D-319E753EDB55}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="36.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>190</v>
+      </c>
+      <c r="H1" s="57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" s="56" t="s">
+        <v>193</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>194</v>
+      </c>
+      <c r="H2" s="56">
+        <v>1234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109F5396-AEFE-4B69-A083-6662A47FD65A}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="29">
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DCD7318-A5F3-4498-8096-038B67B25CA0}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.7265625" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>197</v>
+      </c>
+      <c r="H1" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1" s="57" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>201</v>
+      </c>
+      <c r="H2" s="56">
+        <v>10000</v>
+      </c>
+      <c r="I2" s="58" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F19261-6837-44AB-8CDF-ACF0A2220A25}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="13">
+        <v>1.23456789012345E+28</v>
+      </c>
+      <c r="E2" s="15">
+        <v>1.23123212312321E+24</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="12">
+        <v>18</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="17">
+        <v>45644</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
27th commit - bank regularization summary
27th commit - bank regularization summary
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.6.206\Users\yadhukrishnan.p\Documents\GitHub\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04CF3EC-8F86-4D43-8FE5-9CC5ED917663}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41196FA-0FD0-45A6-8F65-52C407E9B374}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="6" activeTab="7" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="6" activeTab="8" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Disposition_master" sheetId="3" r:id="rId1"/>
@@ -21,15 +21,16 @@
     <sheet name="CoreAlertsMaskAcAndMaskingAutho" sheetId="17" r:id="rId6"/>
     <sheet name="AgentAccountAllocation" sheetId="18" r:id="rId7"/>
     <sheet name="CoreBankAllocationSummary" sheetId="19" r:id="rId8"/>
-    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId9"/>
-    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId10"/>
-    <sheet name="CoreUserManagement" sheetId="6" r:id="rId11"/>
-    <sheet name="CoreHOUserCreation" sheetId="7" r:id="rId12"/>
-    <sheet name="CA-AddNewAgent" sheetId="8" r:id="rId13"/>
-    <sheet name="Core_Regularization_Summary" sheetId="9" r:id="rId14"/>
-    <sheet name="CollectionAgencyDisposition" sheetId="10" r:id="rId15"/>
-    <sheet name="CA-AgentAccountAllocation" sheetId="11" r:id="rId16"/>
-    <sheet name="Core_LoginBannerConfig" sheetId="12" r:id="rId17"/>
+    <sheet name="CoreBankRegularizationSummary" sheetId="20" r:id="rId9"/>
+    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId10"/>
+    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId11"/>
+    <sheet name="CoreUserManagement" sheetId="6" r:id="rId12"/>
+    <sheet name="CoreHOUserCreation" sheetId="7" r:id="rId13"/>
+    <sheet name="CA-AddNewAgent" sheetId="8" r:id="rId14"/>
+    <sheet name="Core_Regularization_Summary" sheetId="9" r:id="rId15"/>
+    <sheet name="CollectionAgencyDisposition" sheetId="10" r:id="rId16"/>
+    <sheet name="CA-AgentAccountAllocation" sheetId="11" r:id="rId17"/>
+    <sheet name="Core_LoginBannerConfig" sheetId="12" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="203">
   <si>
     <t>Run</t>
   </si>
@@ -660,6 +661,9 @@
   </si>
   <si>
     <t>&lt;</t>
+  </si>
+  <si>
+    <t>CoreBankRegularizationSummary</t>
   </si>
 </sst>
 </file>
@@ -1411,6 +1415,103 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F19261-6837-44AB-8CDF-ACF0A2220A25}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="13">
+        <v>1.23456789012345E+28</v>
+      </c>
+      <c r="E2" s="15">
+        <v>1.23123212312321E+24</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="12">
+        <v>18</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="17">
+        <v>45644</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCC895A-2382-45F5-A8F1-2814E48093FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1465,7 +1566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD0DAF-92F9-4A53-BD4C-11CDE669575B}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
@@ -1671,7 +1772,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1090DB4-E483-4C4D-8367-1410BDACF1EB}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1744,7 +1845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB84F0AE-8762-4FD5-92CA-A4BB37675E67}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1792,7 +1893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89943E99-F0EA-477A-BC49-972CD3C95FD8}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1862,7 +1963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE214A7F-1CCD-473B-9D90-2C8A2FFCDD67}">
   <dimension ref="A1:S2"/>
   <sheetViews>
@@ -2004,7 +2105,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502A90A9-AB89-4C76-BF21-0726E83DFEAA}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -2093,7 +2194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319A2FA0-C188-4BFC-B422-FA837B3784A7}">
   <dimension ref="A1:R2"/>
   <sheetViews>
@@ -2574,8 +2675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DCD7318-A5F3-4498-8096-038B67B25CA0}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2654,98 +2755,49 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F19261-6837-44AB-8CDF-ACF0A2220A25}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6993FB2D-6400-4A1B-8C97-912FD43C6B86}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="C1" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="53" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="13">
-        <v>1.23456789012345E+28</v>
-      </c>
-      <c r="E2" s="15">
-        <v>1.23123212312321E+24</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="12">
-        <v>18</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" s="17">
-        <v>45644</v>
+      <c r="C2" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit for Test data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationBeacon\GitHub_Beacon_FCM_Master\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50181411-C936-49C6-B075-587E422ACE87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED921E10-F0C6-4553-904B-13D2DA461FAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="CallCenter" sheetId="8" r:id="rId1"/>
-    <sheet name="AddNewAgent" sheetId="7" r:id="rId2"/>
-    <sheet name="Disposition_master" sheetId="3" r:id="rId3"/>
-    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId4"/>
-    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId5"/>
-    <sheet name="CoreUserManagement" sheetId="6" r:id="rId6"/>
+    <sheet name="AddAgency" sheetId="9" r:id="rId2"/>
+    <sheet name="AddNewAgent" sheetId="7" r:id="rId3"/>
+    <sheet name="Disposition_master" sheetId="3" r:id="rId4"/>
+    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId5"/>
+    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId6"/>
+    <sheet name="CoreUserManagement" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="102">
   <si>
     <t>Run</t>
   </si>
@@ -344,6 +345,12 @@
   <si>
     <t>CallCenter</t>
   </si>
+  <si>
+    <t>CoreAddAgency</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
 </sst>
 </file>
 
@@ -352,7 +359,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,6 +390,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -457,7 +470,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -521,6 +534,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -839,7 +853,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,11 +896,60 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687623D0-D57B-4166-B594-4AF2CAA6F773}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1379A03F-0BDE-4AFB-B2D4-4C2EF4A1030A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,7 +993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067DCD9D-336F-4B7B-9363-04AE9D95019D}">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -1091,7 +1154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F19261-6837-44AB-8CDF-ACF0A2220A25}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1188,7 +1251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCC895A-2382-45F5-A8F1-2814E48093FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1243,7 +1306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD0DAF-92F9-4A53-BD4C-11CDE669575B}">
   <dimension ref="A1:Z2"/>
   <sheetViews>

</xml_diff>

<commit_message>
2nd Commit #View Template List
2nd Commit #View Template List
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megha.zarkar\Documents\GitHub\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5438D6-52F7-4C91-974F-82DB4982F06F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0568BC54-0D02-479D-BEDB-03AAA2EEDE52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15930" windowHeight="2805" tabRatio="597" activeTab="3" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="137">
   <si>
     <t>Run</t>
   </si>
@@ -450,6 +450,12 @@
   </si>
   <si>
     <t>Q1</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Yes,No</t>
   </si>
 </sst>
 </file>
@@ -1317,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280FE8FD-D2BB-4A01-A509-A942B9BAD8DD}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,9 +1334,10 @@
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
@@ -1343,8 +1350,11 @@
       <c r="D1" s="21" t="s">
         <v>133</v>
       </c>
+      <c r="E1" s="21" t="s">
+        <v>135</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>130</v>
       </c>
@@ -1356,6 +1366,9 @@
       </c>
       <c r="D2" s="22" t="s">
         <v>134</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit update forAddAgency Page
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationBeacon\GitHub_Beacon_FCM_Master\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED921E10-F0C6-4553-904B-13D2DA461FAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F7799A-7F7B-46D1-A3C9-489049C9B1E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="CallCenter" sheetId="8" r:id="rId1"/>
-    <sheet name="AddAgency" sheetId="9" r:id="rId2"/>
-    <sheet name="AddNewAgent" sheetId="7" r:id="rId3"/>
-    <sheet name="Disposition_master" sheetId="3" r:id="rId4"/>
-    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId5"/>
-    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId6"/>
-    <sheet name="CoreUserManagement" sheetId="6" r:id="rId7"/>
+    <sheet name="AddAgencyList" sheetId="10" r:id="rId2"/>
+    <sheet name="AddAgency" sheetId="9" r:id="rId3"/>
+    <sheet name="AddNewAgent" sheetId="7" r:id="rId4"/>
+    <sheet name="Disposition_master" sheetId="3" r:id="rId5"/>
+    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId6"/>
+    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId7"/>
+    <sheet name="CoreUserManagement" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="105">
   <si>
     <t>Run</t>
   </si>
@@ -351,6 +352,15 @@
   <si>
     <t>Zone</t>
   </si>
+  <si>
+    <t>CoreAddAgencyList</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Update Adress</t>
+  </si>
 </sst>
 </file>
 
@@ -359,7 +369,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,6 +405,12 @@
       <sz val="9"/>
       <color rgb="FF1F1F1F"/>
       <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
       <family val="3"/>
     </font>
   </fonts>
@@ -470,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -535,6 +551,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -896,10 +913,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B659BFA7-C6D0-4B60-A4EE-B5E1B75045A7}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687623D0-D57B-4166-B594-4AF2CAA6F773}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -944,7 +1020,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1379A03F-0BDE-4AFB-B2D4-4C2EF4A1030A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -993,7 +1069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067DCD9D-336F-4B7B-9363-04AE9D95019D}">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -1154,7 +1230,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F19261-6837-44AB-8CDF-ACF0A2220A25}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1251,7 +1327,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCC895A-2382-45F5-A8F1-2814E48093FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1306,7 +1382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD0DAF-92F9-4A53-BD4C-11CDE669575B}">
   <dimension ref="A1:Z2"/>
   <sheetViews>

</xml_diff>

<commit_message>
for Add Agency List
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationBeacon\GitHub_Beacon_FCM_Master\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F7799A-7F7B-46D1-A3C9-489049C9B1E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE772C7-55C5-4F1E-B4C9-2C054965448A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="107">
   <si>
     <t>Run</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t>Update Adress</t>
+  </si>
+  <si>
+    <t>AgencyCreatedInAddAgencyFlow</t>
+  </si>
+  <si>
+    <t>ATMNAgencykpm</t>
   </si>
 </sst>
 </file>
@@ -914,18 +920,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B659BFA7-C6D0-4B60-A4EE-B5E1B75045A7}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
@@ -944,8 +951,11 @@
       <c r="F1" s="28" t="s">
         <v>103</v>
       </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
@@ -963,6 +973,9 @@
       </c>
       <c r="F2" t="s">
         <v>104</v>
+      </c>
+      <c r="G2" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit for AddAgency and Agency List
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationBeacon\GitHub_Beacon_FCM_Master\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE772C7-55C5-4F1E-B4C9-2C054965448A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25F81E5-9356-4F57-A8D4-6B1C2A21A003}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="109">
   <si>
     <t>Run</t>
   </si>
@@ -365,7 +365,13 @@
     <t>AgencyCreatedInAddAgencyFlow</t>
   </si>
   <si>
-    <t>ATMNAgencykpm</t>
+    <t>ATMNAgencybBx</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -492,7 +498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -558,6 +564,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -920,19 +929,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B659BFA7-C6D0-4B60-A4EE-B5E1B75045A7}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
@@ -951,11 +961,17 @@
       <c r="F1" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="29" t="s">
         <v>105</v>
       </c>
+      <c r="H1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Updated the code with keep button logic
Updated the code with keep button logic
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Beacon_Automation\Latest\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37049A0A-B8AA-4CF9-835B-2740BF5C624D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AF6492-9FF3-4572-B3EA-7A43A46F1543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="5" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
@@ -18,7 +18,8 @@
     <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId3"/>
     <sheet name="CoreUserManagement" sheetId="6" r:id="rId4"/>
     <sheet name="CoreHOUserCreation" sheetId="7" r:id="rId5"/>
-    <sheet name="Allocation_Summary" sheetId="8" r:id="rId6"/>
+    <sheet name="CA-AllocationSummary" sheetId="10" r:id="rId6"/>
+    <sheet name="Allocation_Summary" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="108">
   <si>
     <t>Run</t>
   </si>
@@ -364,6 +365,9 @@
   </si>
   <si>
     <t>Allocation Summary</t>
+  </si>
+  <si>
+    <t>CA-AllocationSummary</t>
   </si>
 </sst>
 </file>
@@ -1462,10 +1466,64 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F01D77-7FCD-4325-93DB-B141ADAEEE17}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D1F0F7-F5FE-4E2D-924E-0FAFB668A140}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Commit for Agent List
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,28 +3,29 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationBeacon\GitHub_Beacon_FCM_Master\BeaconFCM_SJ\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25F81E5-9356-4F57-A8D4-6B1C2A21A003}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E75F7D-6686-4509-9B7F-B5A1008E0D90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{37B91979-A2CD-4275-8B46-28CAE73357A2}"/>
   </bookViews>
   <sheets>
     <sheet name="CallCenter" sheetId="8" r:id="rId1"/>
-    <sheet name="AddAgencyList" sheetId="10" r:id="rId2"/>
-    <sheet name="AddAgency" sheetId="9" r:id="rId3"/>
-    <sheet name="AddNewAgent" sheetId="7" r:id="rId4"/>
-    <sheet name="Disposition_master" sheetId="3" r:id="rId5"/>
-    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId6"/>
-    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId7"/>
-    <sheet name="CoreUserManagement" sheetId="6" r:id="rId8"/>
+    <sheet name="CoreAgentList" sheetId="11" r:id="rId2"/>
+    <sheet name="AddAgencyList" sheetId="10" r:id="rId3"/>
+    <sheet name="AddAgency" sheetId="9" r:id="rId4"/>
+    <sheet name="AddNewAgent" sheetId="7" r:id="rId5"/>
+    <sheet name="Disposition_master" sheetId="3" r:id="rId6"/>
+    <sheet name="Updation_of_Disposition" sheetId="4" r:id="rId7"/>
+    <sheet name="CollectionAgencyRoleManagement" sheetId="5" r:id="rId8"/>
+    <sheet name="CoreUserManagement" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="175">
   <si>
     <t>Run</t>
   </si>
@@ -365,13 +366,211 @@
     <t>AgencyCreatedInAddAgencyFlow</t>
   </si>
   <si>
-    <t>ATMNAgencybBx</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>ATMNAgencywmf</t>
+  </si>
+  <si>
+    <t>AGY0002444</t>
+  </si>
+  <si>
+    <t>QadAEO</t>
+  </si>
+  <si>
+    <t>CoreAddAgentList</t>
+  </si>
+  <si>
+    <t>Agent Name</t>
+  </si>
+  <si>
+    <t>Agent Password</t>
+  </si>
+  <si>
+    <t>AGY0002447</t>
+  </si>
+  <si>
+    <t>gn3l4%</t>
+  </si>
+  <si>
+    <t>AGY0002450</t>
+  </si>
+  <si>
+    <t>!pva22</t>
+  </si>
+  <si>
+    <t>AGY0002451</t>
+  </si>
+  <si>
+    <t>1%8B1N</t>
+  </si>
+  <si>
+    <t>AGY0002452</t>
+  </si>
+  <si>
+    <t>%1Yd2E</t>
+  </si>
+  <si>
+    <t>AGY0002453</t>
+  </si>
+  <si>
+    <t>3V1%as</t>
+  </si>
+  <si>
+    <t>AGY0002454</t>
+  </si>
+  <si>
+    <t>a@2aC8</t>
+  </si>
+  <si>
+    <t>AGY0002455</t>
+  </si>
+  <si>
+    <t>BD!26b</t>
+  </si>
+  <si>
+    <t>ATMNAgencyVNh</t>
+  </si>
+  <si>
+    <t>AGY0002456</t>
+  </si>
+  <si>
+    <t>9tWme5</t>
+  </si>
+  <si>
+    <t>ATMNAgencyZd5</t>
+  </si>
+  <si>
+    <t>AGY0002457</t>
+  </si>
+  <si>
+    <t>VJ6FQx</t>
+  </si>
+  <si>
+    <t>ATMNAgency4G0</t>
+  </si>
+  <si>
+    <t>ATMNAgencyfuO</t>
+  </si>
+  <si>
+    <t>AGY0002459</t>
+  </si>
+  <si>
+    <t>fgP8xD</t>
+  </si>
+  <si>
+    <t>ATMNAgencydMI</t>
+  </si>
+  <si>
+    <t>AGY0002460</t>
+  </si>
+  <si>
+    <t>aurVVg</t>
+  </si>
+  <si>
+    <t>ATMNAgencyP4r</t>
+  </si>
+  <si>
+    <t>AGY0002461</t>
+  </si>
+  <si>
+    <t>5ojbV3</t>
+  </si>
+  <si>
+    <t>ATMNAgencyUr2</t>
+  </si>
+  <si>
+    <t>AGY0002462</t>
+  </si>
+  <si>
+    <t>94YaHd</t>
+  </si>
+  <si>
+    <t>ATMNAgencygfw</t>
+  </si>
+  <si>
+    <t>AGY0002463</t>
+  </si>
+  <si>
+    <t>T4qYjM</t>
+  </si>
+  <si>
+    <t>AGY0002464</t>
+  </si>
+  <si>
+    <t>Do1Y@7</t>
+  </si>
+  <si>
+    <t>ATMNAgency8HH</t>
+  </si>
+  <si>
+    <t>AGY0002465</t>
+  </si>
+  <si>
+    <t>nEq1d4</t>
+  </si>
+  <si>
+    <t>ATMNAgencyihH</t>
+  </si>
+  <si>
+    <t>AGY0002466</t>
+  </si>
+  <si>
+    <t>3n1AFC</t>
+  </si>
+  <si>
+    <t>AGY0002467</t>
+  </si>
+  <si>
+    <t>v5T7R#</t>
+  </si>
+  <si>
+    <t>ATMNAgencyRrW</t>
+  </si>
+  <si>
+    <t>AGY0002468</t>
+  </si>
+  <si>
+    <t>7EnANU</t>
+  </si>
+  <si>
+    <t>AGY0002469</t>
+  </si>
+  <si>
+    <t>g!37s2</t>
+  </si>
+  <si>
+    <t>AGY0002470</t>
+  </si>
+  <si>
+    <t>QFzl7I</t>
+  </si>
+  <si>
+    <t>AGY0002471</t>
+  </si>
+  <si>
+    <t>13jmb3</t>
+  </si>
+  <si>
+    <t>AGY0002472</t>
+  </si>
+  <si>
+    <t>zCssyr</t>
+  </si>
+  <si>
+    <t>AGY0002473</t>
+  </si>
+  <si>
+    <t>z16ZvB</t>
+  </si>
+  <si>
+    <t>AGY0002474</t>
+  </si>
+  <si>
+    <t>MXMpms</t>
   </si>
 </sst>
 </file>
@@ -890,10 +1089,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.7109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="4.42578125"/>
+    <col min="4" max="4" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -928,18 +1127,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C286CB-AEE3-4F9C-BEDF-B5181A1244C5}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.7109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="4.42578125"/>
+    <col min="4" max="4" customWidth="true" width="18.0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B659BFA7-C6D0-4B60-A4EE-B5E1B75045A7}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="14.140625"/>
+    <col min="6" max="6" customWidth="true" width="13.85546875"/>
+    <col min="7" max="7" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -955,7 +1209,7 @@
       <c r="D1" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>72</v>
       </c>
       <c r="F1" s="28" t="s">
@@ -964,11 +1218,11 @@
       <c r="G1" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="I1" t="s" s="0">
         <v>107</v>
-      </c>
-      <c r="I1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -987,11 +1241,17 @@
       <c r="E2" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="G2" t="s">
-        <v>106</v>
+      <c r="G2" t="s" s="0">
+        <v>160</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>173</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1000,7 +1260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687623D0-D57B-4166-B594-4AF2CAA6F773}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1023,7 +1283,7 @@
       <c r="D1" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>72</v>
       </c>
     </row>
@@ -1049,7 +1309,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1379A03F-0BDE-4AFB-B2D4-4C2EF4A1030A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1059,10 +1319,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.7109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="4.42578125"/>
+    <col min="4" max="4" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,7 +1358,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067DCD9D-336F-4B7B-9363-04AE9D95019D}">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -1108,26 +1368,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.7109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="4.42578125"/>
+    <col min="4" max="4" customWidth="true" width="18.0"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.85546875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.0"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="41.5703125"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="29.28515625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="42.85546875"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.7109375"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="42.85546875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="27.85546875"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="13.28515625"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.5703125"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="20.5703125"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="18.85546875"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="28.85546875"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="45.85546875"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="40.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -1259,7 +1519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F19261-6837-44AB-8CDF-ACF0A2220A25}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -1269,15 +1529,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.85546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.85546875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="26.140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.7109375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.140625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="4.85546875"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1356,7 +1616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCC895A-2382-45F5-A8F1-2814E48093FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1366,10 +1626,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.42578125"/>
+    <col min="3" max="3" customWidth="true" width="16.5703125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125"/>
+    <col min="5" max="5" customWidth="true" width="26.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1411,7 +1671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD0DAF-92F9-4A53-BD4C-11CDE669575B}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
@@ -1419,30 +1679,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.7109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="5.7109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.85546875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.5703125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.5703125"/>
+    <col min="8" max="10" bestFit="true" customWidth="true" width="16.5703125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.140625"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="14.85546875"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="19.140625"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="17.7109375"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="16.5703125"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="19.42578125"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="17.42578125"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="22.42578125"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="7.85546875"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="6.42578125"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="15.140625"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="7.42578125"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="23.7109375"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="17.7109375"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="9.85546875"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="10.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>